<commit_message>
updated results for text input field test cases
</commit_message>
<xml_diff>
--- a/TestDocuments/TestCases.xlsx
+++ b/TestDocuments/TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quality Assurance\Workings\Automated Test\RahulshettyPractice\RahulShettyAcademyAutomatedTest\Test Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quality Assurance\Workings\Automated Test\RahulshettyPractice\RahulShettyAcademyAutomatedTest\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F7B170-AD8B-47F7-BDDB-18817DD88762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C14C8F-2AFF-4740-BE44-D897E0C42C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="136">
   <si>
     <t>Functional Testing</t>
   </si>
@@ -447,6 +447,9 @@
   </si>
   <si>
     <t>https://prnt.sc/LQYc57o9pniS</t>
+  </si>
+  <si>
+    <t>Verifying text input field heading</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1324,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1529,9 +1532,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1664,6 +1664,110 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="37" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1674,100 +1778,6 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1786,15 +1796,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="37" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2118,10 +2121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CD4380-2153-411E-9E75-935A9463F7F9}">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2132,107 +2135,107 @@
     <col min="4" max="4" width="30.28515625" style="58" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="60.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="71.28515625" style="119" customWidth="1"/>
+    <col min="7" max="7" width="71.28515625" style="118" customWidth="1"/>
     <col min="8" max="11" width="22.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="26.42578125" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="157" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="104" t="s">
+      <c r="B1" s="158"/>
+      <c r="C1" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="114"/>
-      <c r="K1" s="120" t="s">
+      <c r="G1" s="113"/>
+      <c r="K1" s="155" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="121"/>
+      <c r="L1" s="156"/>
     </row>
     <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="105" t="s">
+      <c r="B2" s="158"/>
+      <c r="C2" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="114"/>
+      <c r="G2" s="113"/>
       <c r="K2" s="32" t="s">
         <v>22</v>
       </c>
       <c r="L2" s="29">
-        <f>COUNTIF(L8:L363,"Passed")</f>
-        <v>6</v>
+        <f>COUNTIF(L8:L364,"Passed")</f>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="157" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="105" t="s">
+      <c r="B3" s="158"/>
+      <c r="C3" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="114"/>
+      <c r="G3" s="113"/>
       <c r="K3" s="31" t="s">
         <v>20</v>
       </c>
       <c r="L3" s="29">
-        <f>COUNTIF(L8:L710,"Failed")</f>
+        <f>COUNTIF(L8:L711,"Failed")</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="129"/>
-      <c r="C4" s="105" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="114"/>
+      <c r="G4" s="113"/>
       <c r="K4" s="30" t="s">
         <v>17</v>
       </c>
       <c r="L4" s="29">
-        <f>COUNTIF(L7:L710,"Not Executed")</f>
+        <f>COUNTIF(L7:L711,"Not Executed")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="137" t="s">
+      <c r="B5" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="138"/>
+      <c r="C5" s="140"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" s="115"/>
+      <c r="G5" s="114"/>
       <c r="H5"/>
       <c r="K5" s="28" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="27">
-        <f>COUNTIF(L7:L710,"Out of Scope")</f>
+        <f>COUNTIF(L7:L711,"Out of Scope")</f>
         <v>0</v>
       </c>
     </row>
@@ -2240,17 +2243,17 @@
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="87"/>
+      <c r="D6" s="86"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
-      <c r="G6" s="116"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="25"/>
       <c r="K6" s="24" t="s">
         <v>13</v>
       </c>
       <c r="L6" s="23">
         <f>SUM(L2:L5)</f>
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2272,7 +2275,7 @@
       <c r="F7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="112" t="s">
+      <c r="G7" s="111" t="s">
         <v>28</v>
       </c>
       <c r="H7" s="21" t="s">
@@ -2292,20 +2295,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="93">
+      <c r="A8" s="92">
         <v>1</v>
       </c>
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="130" t="s">
+      <c r="C8" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="133" t="s">
+      <c r="D8" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="139"/>
-      <c r="F8" s="106" t="s">
+      <c r="E8" s="141"/>
+      <c r="F8" s="105" t="s">
         <v>84</v>
       </c>
       <c r="G8" s="63" t="s">
@@ -2314,26 +2317,26 @@
       <c r="H8" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="I8" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="J8" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="K8" s="162" t="s">
+      <c r="I8" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K8" s="120" t="s">
         <v>132</v>
       </c>
       <c r="L8" s="42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="102" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="93"/>
-      <c r="B9" s="126"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="134"/>
-      <c r="E9" s="140"/>
-      <c r="F9" s="106" t="s">
+    <row r="9" spans="1:12" s="101" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="92"/>
+      <c r="B9" s="130"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="105" t="s">
         <v>125</v>
       </c>
       <c r="G9" s="63" t="s">
@@ -2342,13 +2345,13 @@
       <c r="H9" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="I9" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="J9" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="K9" s="162" t="s">
+      <c r="I9" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J9" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K9" s="120" t="s">
         <v>132</v>
       </c>
       <c r="L9" s="42" t="s">
@@ -2356,29 +2359,29 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="93">
+      <c r="A10" s="92">
         <v>2</v>
       </c>
-      <c r="B10" s="126"/>
-      <c r="C10" s="131"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="140"/>
-      <c r="F10" s="107" t="s">
+      <c r="B10" s="130"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="113" t="s">
+      <c r="G10" s="112" t="s">
         <v>81</v>
       </c>
       <c r="H10" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="I10" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="J10" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="K10" s="162" t="s">
+      <c r="I10" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" s="120" t="s">
         <v>132</v>
       </c>
       <c r="L10" s="42" t="s">
@@ -2386,27 +2389,27 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="93"/>
-      <c r="B11" s="126"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="108" t="s">
+      <c r="A11" s="92"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="142"/>
+      <c r="F11" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="113" t="s">
+      <c r="G11" s="112" t="s">
         <v>82</v>
       </c>
       <c r="H11" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="I11" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="J11" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="K11" s="162" t="s">
+      <c r="I11" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J11" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K11" s="120" t="s">
         <v>132</v>
       </c>
       <c r="L11" s="42" t="s">
@@ -2414,29 +2417,29 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="93">
+      <c r="A12" s="92">
         <v>3</v>
       </c>
-      <c r="B12" s="126"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="109" t="s">
+      <c r="B12" s="130"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="142"/>
+      <c r="F12" s="108" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="117" t="s">
+      <c r="G12" s="116" t="s">
         <v>83</v>
       </c>
       <c r="H12" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="I12" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="J12" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="K12" s="162" t="s">
+      <c r="I12" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J12" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" s="120" t="s">
         <v>132</v>
       </c>
       <c r="L12" s="42" t="s">
@@ -2444,44 +2447,44 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="93"/>
-      <c r="B13" s="126"/>
-      <c r="C13" s="148" t="s">
+      <c r="A13" s="92"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="150" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="135"/>
-      <c r="E13" s="140"/>
-      <c r="F13" s="110" t="s">
+      <c r="D13" s="137"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="118" t="s">
+      <c r="G13" s="117" t="s">
         <v>106</v>
       </c>
       <c r="H13" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="I13" s="162" t="s">
+      <c r="I13" s="120" t="s">
         <v>132</v>
       </c>
       <c r="J13" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="K13" s="164" t="s">
+      <c r="K13" s="122" t="s">
         <v>134</v>
       </c>
-      <c r="L13" s="163" t="s">
+      <c r="L13" s="121" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="93">
+      <c r="A14" s="92">
         <v>4</v>
       </c>
-      <c r="B14" s="126"/>
-      <c r="C14" s="149"/>
-      <c r="D14" s="136"/>
-      <c r="E14" s="141"/>
-      <c r="F14" s="111" t="s">
+      <c r="B14" s="130"/>
+      <c r="C14" s="151"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="143"/>
+      <c r="F14" s="110" t="s">
         <v>89</v>
       </c>
       <c r="G14" s="59" t="s">
@@ -2490,13 +2493,13 @@
       <c r="H14" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="I14" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="J14" s="162" t="s">
-        <v>132</v>
-      </c>
-      <c r="K14" s="162" t="s">
+      <c r="I14" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J14" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K14" s="120" t="s">
         <v>132</v>
       </c>
       <c r="L14" s="67" t="s">
@@ -2504,222 +2507,300 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="93">
+      <c r="A15" s="92">
         <v>5</v>
       </c>
-      <c r="B15" s="126"/>
-      <c r="C15" s="130" t="s">
+      <c r="B15" s="130"/>
+      <c r="C15" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="133" t="s">
+      <c r="D15" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="142"/>
+      <c r="E15" s="144"/>
       <c r="F15" s="50" t="s">
         <v>90</v>
       </c>
       <c r="G15" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="36"/>
-    </row>
-    <row r="16" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="93">
+      <c r="H15" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J15" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K15" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="L15" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="119" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="92"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="125"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J16" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K16" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="L16" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="92">
         <v>6</v>
       </c>
-      <c r="B16" s="126"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="12" t="s">
+      <c r="B17" s="130"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G17" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="93">
+      <c r="H17" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I17" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J17" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K17" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="L17" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="92">
         <v>7</v>
       </c>
-      <c r="B17" s="126"/>
-      <c r="C17" s="132"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="143"/>
-      <c r="F17" s="45" t="s">
+      <c r="B18" s="130"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="145"/>
+      <c r="F18" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="46" t="s">
+      <c r="G18" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="93">
+      <c r="H18" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I18" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J18" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K18" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="L18" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="92">
         <v>8</v>
       </c>
-      <c r="B18" s="126"/>
-      <c r="C18" s="130" t="s">
+      <c r="B19" s="130"/>
+      <c r="C19" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="134"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="37" t="s">
+      <c r="D19" s="136"/>
+      <c r="E19" s="145"/>
+      <c r="F19" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="63" t="s">
+      <c r="G19" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="42"/>
-    </row>
-    <row r="19" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="93"/>
-      <c r="B19" s="126"/>
-      <c r="C19" s="131"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="143"/>
-      <c r="F19" s="45" t="s">
+      <c r="H19" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J19" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K19" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="L19" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="92"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="145"/>
+      <c r="F20" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="59" t="s">
+      <c r="G20" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="75"/>
-    </row>
-    <row r="20" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="93"/>
-      <c r="B20" s="126"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="45" t="s">
+      <c r="H20" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I20" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J20" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K20" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="L20" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="92"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="145"/>
+      <c r="F21" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="G21" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="75"/>
-    </row>
-    <row r="21" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="93">
+      <c r="H21" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J21" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K21" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="L21" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="92">
         <v>9</v>
       </c>
-      <c r="B21" s="126"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="150"/>
-      <c r="E21" s="144"/>
-      <c r="F21" s="45" t="s">
+      <c r="B22" s="130"/>
+      <c r="C22" s="124"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="73" t="s">
+      <c r="G22" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93">
+      <c r="H22" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I22" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J22" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="K22" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="L22" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="92">
         <v>10</v>
       </c>
-      <c r="B22" s="126"/>
-      <c r="C22" s="130" t="s">
+      <c r="B23" s="130"/>
+      <c r="C23" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="151" t="s">
+      <c r="D23" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="145"/>
-      <c r="F22" s="37" t="s">
+      <c r="E23" s="147"/>
+      <c r="F23" s="37" t="s">
         <v>96</v>
-      </c>
-      <c r="G22" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="42"/>
-    </row>
-    <row r="23" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="93"/>
-      <c r="B23" s="126"/>
-      <c r="C23" s="131"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="37" t="s">
-        <v>97</v>
       </c>
       <c r="G23" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="36"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="42"/>
     </row>
     <row r="24" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="93">
+      <c r="A24" s="92"/>
+      <c r="B24" s="130"/>
+      <c r="C24" s="125"/>
+      <c r="D24" s="127"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="36"/>
+    </row>
+    <row r="25" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="92">
         <v>11</v>
       </c>
-      <c r="B24" s="126"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="152"/>
-      <c r="E24" s="146"/>
-      <c r="F24" s="15" t="s">
+      <c r="B25" s="130"/>
+      <c r="C25" s="125"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="148"/>
+      <c r="F25" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="G24" s="113" t="s">
+      <c r="G25" s="112" t="s">
         <v>81</v>
-      </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="93">
-        <v>12</v>
-      </c>
-      <c r="B25" s="126"/>
-      <c r="C25" s="131"/>
-      <c r="D25" s="152"/>
-      <c r="E25" s="146"/>
-      <c r="F25" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
@@ -2728,104 +2809,104 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="93">
+      <c r="A26" s="92">
+        <v>12</v>
+      </c>
+      <c r="B26" s="130"/>
+      <c r="C26" s="125"/>
+      <c r="D26" s="127"/>
+      <c r="E26" s="148"/>
+      <c r="F26" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="7"/>
+    </row>
+    <row r="27" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="92">
         <v>13</v>
       </c>
-      <c r="B26" s="126"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="146"/>
-      <c r="F26" s="68" t="s">
+      <c r="B27" s="130"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="127"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="46" t="s">
+      <c r="G27" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="93">
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="92">
         <v>14</v>
       </c>
-      <c r="B27" s="126"/>
-      <c r="C27" s="70" t="s">
+      <c r="B28" s="130"/>
+      <c r="C28" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="153"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="71" t="s">
+      <c r="D28" s="128"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="46" t="s">
+      <c r="G28" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="62"/>
-    </row>
-    <row r="28" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="93">
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="61"/>
+      <c r="L28" s="62"/>
+    </row>
+    <row r="29" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="92">
         <v>15</v>
       </c>
-      <c r="B28" s="126"/>
-      <c r="C28" s="130" t="s">
+      <c r="B29" s="130"/>
+      <c r="C29" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="151" t="s">
+      <c r="D29" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="56"/>
-      <c r="F28" s="37" t="s">
+      <c r="E29" s="56"/>
+      <c r="F29" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="G28" s="40" t="s">
+      <c r="G29" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="42"/>
-    </row>
-    <row r="29" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="93">
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="42"/>
+    </row>
+    <row r="30" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="92">
         <v>16</v>
       </c>
-      <c r="B29" s="126"/>
-      <c r="C29" s="131"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="15" t="s">
+      <c r="B30" s="130"/>
+      <c r="C30" s="125"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G30" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="7"/>
-    </row>
-    <row r="30" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="93">
-        <v>17</v>
-      </c>
-      <c r="B30" s="126"/>
-      <c r="C30" s="131"/>
-      <c r="D30" s="152"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>82</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
@@ -2834,102 +2915,100 @@
       <c r="L30" s="7"/>
     </row>
     <row r="31" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="94">
-        <v>18</v>
-      </c>
-      <c r="B31" s="126"/>
-      <c r="C31" s="131"/>
-      <c r="D31" s="152"/>
+      <c r="A31" s="92">
+        <v>17</v>
+      </c>
+      <c r="B31" s="130"/>
+      <c r="C31" s="125"/>
+      <c r="D31" s="127"/>
       <c r="E31" s="43"/>
       <c r="F31" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="11"/>
       <c r="K31" s="9"/>
       <c r="L31" s="7"/>
     </row>
     <row r="32" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="94">
+      <c r="A32" s="93">
+        <v>18</v>
+      </c>
+      <c r="B32" s="130"/>
+      <c r="C32" s="125"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="7"/>
+    </row>
+    <row r="33" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="93">
         <v>19</v>
       </c>
-      <c r="B32" s="126"/>
-      <c r="C32" s="132"/>
-      <c r="D32" s="153"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="68" t="s">
+      <c r="B33" s="130"/>
+      <c r="C33" s="124"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="G32" s="46" t="s">
+      <c r="G33" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="94">
+      <c r="H33" s="6"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="93">
         <v>20</v>
       </c>
-      <c r="B33" s="126"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="151" t="s">
+      <c r="B34" s="130"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="56"/>
-      <c r="F33" s="88" t="s">
+      <c r="E34" s="56"/>
+      <c r="F34" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="G33" s="39" t="s">
+      <c r="G34" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="H33" s="89"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="42"/>
-    </row>
-    <row r="34" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="94">
+      <c r="H34" s="88"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="42"/>
+    </row>
+    <row r="35" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="93">
         <v>21</v>
       </c>
-      <c r="B34" s="126"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="152"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="7"/>
-    </row>
-    <row r="35" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="94">
-        <v>22</v>
-      </c>
-      <c r="B35" s="126"/>
-      <c r="C35" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="152"/>
+      <c r="B35" s="130"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="127"/>
       <c r="E35" s="43"/>
       <c r="F35" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="8"/>
@@ -2938,18 +3017,20 @@
       <c r="L35" s="7"/>
     </row>
     <row r="36" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="94">
-        <v>23</v>
-      </c>
-      <c r="B36" s="126"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="152"/>
+      <c r="A36" s="93">
+        <v>22</v>
+      </c>
+      <c r="B36" s="130"/>
+      <c r="C36" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="127"/>
       <c r="E36" s="43"/>
       <c r="F36" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>120</v>
+        <v>69</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="8"/>
@@ -2958,203 +3039,201 @@
       <c r="L36" s="7"/>
     </row>
     <row r="37" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="94">
+      <c r="A37" s="93">
+        <v>23</v>
+      </c>
+      <c r="B37" s="130"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="127"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="7"/>
+    </row>
+    <row r="38" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="93">
         <v>24</v>
       </c>
-      <c r="B37" s="126"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="153"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="90" t="s">
+      <c r="B38" s="130"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="128"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H37" s="6"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="94">
+      <c r="H38" s="6"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="93">
         <v>25</v>
       </c>
-      <c r="B38" s="126"/>
-      <c r="C38" s="130" t="s">
+      <c r="B39" s="130"/>
+      <c r="C39" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="151" t="s">
+      <c r="D39" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="56"/>
-      <c r="F38" s="57" t="s">
+      <c r="E39" s="56"/>
+      <c r="F39" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="G38" s="40" t="s">
+      <c r="G39" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="H38" s="89"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="42"/>
-    </row>
-    <row r="39" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
-      <c r="B39" s="126"/>
-      <c r="C39" s="132"/>
-      <c r="D39" s="153"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="92" t="s">
+      <c r="H39" s="88"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="42"/>
+    </row>
+    <row r="40" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="93"/>
+      <c r="B40" s="130"/>
+      <c r="C40" s="124"/>
+      <c r="D40" s="128"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="91" t="s">
         <v>74</v>
-      </c>
-      <c r="G39" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="H39" s="97"/>
-      <c r="I39" s="98"/>
-      <c r="J39" s="98"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="52"/>
-    </row>
-    <row r="40" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="94"/>
-      <c r="B40" s="126"/>
-      <c r="C40" s="130" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="154" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" s="56"/>
-      <c r="F40" s="99" t="s">
-        <v>77</v>
       </c>
       <c r="G40" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="H40" s="100"/>
-      <c r="I40" s="101"/>
-      <c r="J40" s="101"/>
-      <c r="K40" s="65"/>
-      <c r="L40" s="66"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="97"/>
+      <c r="J40" s="97"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="52"/>
     </row>
     <row r="41" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="94"/>
-      <c r="B41" s="126"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="155"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="92" t="s">
+      <c r="A41" s="93"/>
+      <c r="B41" s="130"/>
+      <c r="C41" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="153" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="165"/>
+      <c r="F41" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="H41" s="99"/>
+      <c r="I41" s="100"/>
+      <c r="J41" s="100"/>
+      <c r="K41" s="65"/>
+      <c r="L41" s="66"/>
+    </row>
+    <row r="42" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="93"/>
+      <c r="B42" s="130"/>
+      <c r="C42" s="124"/>
+      <c r="D42" s="154"/>
+      <c r="E42" s="166"/>
+      <c r="F42" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="G41" s="59" t="s">
+      <c r="G42" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="H41" s="97"/>
-      <c r="I41" s="98"/>
-      <c r="J41" s="98"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="52"/>
-    </row>
-    <row r="42" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="94"/>
-      <c r="B42" s="126"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="92"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="95"/>
-      <c r="I42" s="96"/>
-      <c r="J42" s="96"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="75"/>
+      <c r="H42" s="96"/>
+      <c r="I42" s="97"/>
+      <c r="J42" s="97"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="52"/>
     </row>
     <row r="43" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="94"/>
-      <c r="B43" s="126"/>
+      <c r="A43" s="93"/>
+      <c r="B43" s="130"/>
       <c r="C43" s="54"/>
       <c r="D43" s="16"/>
       <c r="E43" s="43"/>
-      <c r="F43" s="92"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="95"/>
-      <c r="I43" s="96"/>
-      <c r="J43" s="96"/>
-      <c r="K43" s="74"/>
-      <c r="L43" s="75"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="94"/>
+      <c r="I43" s="95"/>
+      <c r="J43" s="95"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="74"/>
     </row>
     <row r="44" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="94"/>
-      <c r="B44" s="126"/>
+      <c r="A44" s="93"/>
+      <c r="B44" s="130"/>
       <c r="C44" s="54"/>
       <c r="D44" s="16"/>
       <c r="E44" s="43"/>
-      <c r="F44" s="92"/>
+      <c r="F44" s="91"/>
       <c r="G44" s="59"/>
-      <c r="H44" s="95"/>
-      <c r="I44" s="96"/>
-      <c r="J44" s="96"/>
-      <c r="K44" s="74"/>
-      <c r="L44" s="75"/>
+      <c r="H44" s="94"/>
+      <c r="I44" s="95"/>
+      <c r="J44" s="95"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="74"/>
     </row>
     <row r="45" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="94"/>
-      <c r="B45" s="126"/>
+      <c r="A45" s="93"/>
+      <c r="B45" s="130"/>
       <c r="C45" s="54"/>
       <c r="D45" s="16"/>
       <c r="E45" s="43"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="95"/>
-      <c r="I45" s="96"/>
-      <c r="J45" s="96"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="75"/>
+      <c r="F45" s="91"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="95"/>
+      <c r="J45" s="95"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="74"/>
     </row>
     <row r="46" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="94">
+      <c r="A46" s="93"/>
+      <c r="B46" s="130"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="91"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="94"/>
+      <c r="I46" s="95"/>
+      <c r="J46" s="95"/>
+      <c r="K46" s="73"/>
+      <c r="L46" s="74"/>
+    </row>
+    <row r="47" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="93">
         <v>26</v>
       </c>
-      <c r="B46" s="127"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="92"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="3"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="91"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="D28:D32"/>
-    <mergeCell ref="D33:D37"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B8:B46"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D14"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E8:E14"/>
-    <mergeCell ref="E15:E21"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D15:D21"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="D40:D41"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
@@ -3162,14 +3241,36 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B8:B47"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D14"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E8:E14"/>
+    <mergeCell ref="E15:E22"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="D15:D22"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C39:C40"/>
   </mergeCells>
-  <conditionalFormatting sqref="L8:L46">
+  <conditionalFormatting sqref="L8:L47">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="L8:L46" xr:uid="{63BE6CF9-2C90-478B-A7BF-5CBE8DDE97F0}">
+    <dataValidation type="list" allowBlank="1" sqref="L8:L47" xr:uid="{63BE6CF9-2C90-478B-A7BF-5CBE8DDE97F0}">
       <formula1>"Passed,Failed,Not Executed,Out of Scope"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3186,20 +3287,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E83DD8F-1B30-4A24-875F-463EA716463A}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="86" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="85" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" style="77" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" style="76" customWidth="1"/>
     <col min="4" max="14" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="20" t="s">
@@ -3213,248 +3314,248 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="158">
+      <c r="A2" s="161">
         <v>1</v>
       </c>
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="159" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="84"/>
+      <c r="D2" s="83"/>
     </row>
     <row r="3" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="160"/>
-      <c r="B3" s="161"/>
-      <c r="C3" s="80" t="s">
+      <c r="A3" s="163"/>
+      <c r="B3" s="164"/>
+      <c r="C3" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="85"/>
+      <c r="D3" s="84"/>
     </row>
     <row r="4" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="160"/>
-      <c r="B4" s="161"/>
-      <c r="C4" s="80" t="s">
+      <c r="A4" s="163"/>
+      <c r="B4" s="164"/>
+      <c r="C4" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="85"/>
+      <c r="D4" s="84"/>
     </row>
     <row r="5" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="159"/>
-      <c r="B5" s="161"/>
-      <c r="C5" s="80" t="s">
+      <c r="A5" s="162"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="85"/>
+      <c r="D5" s="84"/>
     </row>
     <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="158">
+      <c r="A6" s="161">
         <v>2</v>
       </c>
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="84"/>
+      <c r="D6" s="83"/>
     </row>
     <row r="7" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="160"/>
-      <c r="B7" s="161"/>
-      <c r="C7" s="80" t="s">
+      <c r="A7" s="163"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="85"/>
+      <c r="D7" s="84"/>
     </row>
     <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="160"/>
-      <c r="B8" s="161"/>
-      <c r="C8" s="80" t="s">
+      <c r="A8" s="163"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="85"/>
+      <c r="D8" s="84"/>
     </row>
     <row r="9" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
-      <c r="B9" s="161"/>
-      <c r="C9" s="80" t="s">
+      <c r="A9" s="163"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="85"/>
+      <c r="D9" s="84"/>
     </row>
     <row r="10" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="160"/>
-      <c r="B10" s="161"/>
-      <c r="C10" s="80" t="s">
+      <c r="A10" s="163"/>
+      <c r="B10" s="164"/>
+      <c r="C10" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="85"/>
+      <c r="D10" s="84"/>
     </row>
     <row r="11" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="159"/>
-      <c r="B11" s="161"/>
-      <c r="C11" s="82" t="s">
+      <c r="A11" s="162"/>
+      <c r="B11" s="164"/>
+      <c r="C11" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="85"/>
+      <c r="D11" s="84"/>
     </row>
     <row r="12" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="158">
+      <c r="A12" s="161">
         <v>3</v>
       </c>
-      <c r="B12" s="156" t="s">
+      <c r="B12" s="159" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="79"/>
+      <c r="D12" s="78"/>
     </row>
     <row r="13" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="160"/>
-      <c r="B13" s="161"/>
-      <c r="C13" s="80" t="s">
+      <c r="A13" s="163"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="81"/>
+      <c r="D13" s="80"/>
     </row>
     <row r="14" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="160"/>
-      <c r="B14" s="161"/>
-      <c r="C14" s="80" t="s">
+      <c r="A14" s="163"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="81"/>
+      <c r="D14" s="80"/>
     </row>
     <row r="15" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="160"/>
-      <c r="B15" s="161"/>
-      <c r="C15" s="80" t="s">
+      <c r="A15" s="163"/>
+      <c r="B15" s="164"/>
+      <c r="C15" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="81"/>
+      <c r="D15" s="80"/>
     </row>
     <row r="16" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="159"/>
-      <c r="B16" s="157"/>
-      <c r="C16" s="82" t="s">
+      <c r="A16" s="162"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="83"/>
+      <c r="D16" s="82"/>
     </row>
     <row r="17" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="158">
+      <c r="A17" s="161">
         <v>4</v>
       </c>
-      <c r="B17" s="156" t="s">
+      <c r="B17" s="159" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="78" t="s">
+      <c r="C17" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="79"/>
+      <c r="D17" s="78"/>
     </row>
     <row r="18" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="160"/>
-      <c r="B18" s="161"/>
-      <c r="C18" s="80" t="s">
+      <c r="A18" s="163"/>
+      <c r="B18" s="164"/>
+      <c r="C18" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="81"/>
+      <c r="D18" s="80"/>
     </row>
     <row r="19" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="160"/>
-      <c r="B19" s="161"/>
-      <c r="C19" s="80" t="s">
+      <c r="A19" s="163"/>
+      <c r="B19" s="164"/>
+      <c r="C19" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="81"/>
+      <c r="D19" s="80"/>
     </row>
     <row r="20" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="160"/>
-      <c r="B20" s="161"/>
-      <c r="C20" s="80" t="s">
+      <c r="A20" s="163"/>
+      <c r="B20" s="164"/>
+      <c r="C20" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="81"/>
+      <c r="D20" s="80"/>
     </row>
     <row r="21" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="158">
+      <c r="A21" s="161">
         <v>5</v>
       </c>
-      <c r="B21" s="156" t="s">
+      <c r="B21" s="159" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="78" t="s">
+      <c r="C21" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="79"/>
+      <c r="D21" s="78"/>
     </row>
     <row r="22" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="160"/>
-      <c r="B22" s="161"/>
-      <c r="C22" s="80" t="s">
+      <c r="A22" s="163"/>
+      <c r="B22" s="164"/>
+      <c r="C22" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="81"/>
+      <c r="D22" s="80"/>
     </row>
     <row r="23" spans="1:4" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="159"/>
-      <c r="B23" s="157"/>
-      <c r="C23" s="82" t="s">
+      <c r="A23" s="162"/>
+      <c r="B23" s="160"/>
+      <c r="C23" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="83"/>
+      <c r="D23" s="82"/>
     </row>
     <row r="24" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="158">
+      <c r="A24" s="161">
         <v>5</v>
       </c>
-      <c r="B24" s="156" t="s">
+      <c r="B24" s="159" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="78" t="s">
+      <c r="C24" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="79"/>
+      <c r="D24" s="78"/>
     </row>
     <row r="25" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="160"/>
-      <c r="B25" s="161"/>
-      <c r="C25" s="80" t="s">
+      <c r="A25" s="163"/>
+      <c r="B25" s="164"/>
+      <c r="C25" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="81"/>
+      <c r="D25" s="80"/>
     </row>
     <row r="26" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="159"/>
-      <c r="B26" s="157"/>
-      <c r="C26" s="82" t="s">
+      <c r="A26" s="162"/>
+      <c r="B26" s="160"/>
+      <c r="C26" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="83"/>
+      <c r="D26" s="82"/>
     </row>
     <row r="27" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="158">
+      <c r="A27" s="161">
         <v>6</v>
       </c>
-      <c r="B27" s="156" t="s">
+      <c r="B27" s="159" t="s">
         <v>127</v>
       </c>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="79"/>
+      <c r="D27" s="78"/>
     </row>
     <row r="28" spans="1:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="159"/>
-      <c r="B28" s="157"/>
-      <c r="C28" s="82" t="s">
+      <c r="A28" s="162"/>
+      <c r="B28" s="160"/>
+      <c r="C28" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="83"/>
+      <c r="D28" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
updated test status for dropdown
</commit_message>
<xml_diff>
--- a/TestDocuments/TestCases.xlsx
+++ b/TestDocuments/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quality Assurance\Workings\Automated Test\RahulshettyPractice\RahulShettyAcademyAutomatedTest\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C14C8F-2AFF-4740-BE44-D897E0C42C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9092F9CF-D093-4C88-AB4E-8C82EA98AD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Elements" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="137">
   <si>
     <t>Functional Testing</t>
   </si>
@@ -335,9 +335,6 @@
     <t>Verifying dropdown selection visibility</t>
   </si>
   <si>
-    <t>Verifying dropdown options are visible when selection is clicked</t>
-  </si>
-  <si>
     <t>Verifying dropdown selection options by Label and Value</t>
   </si>
   <si>
@@ -450,6 +447,12 @@
   </si>
   <si>
     <t>Verifying text input field heading</t>
+  </si>
+  <si>
+    <t>Verifying  Multiples options are not selectable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should not be selectable </t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1327,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1420,18 +1423,6 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1458,9 +1449,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1495,15 +1483,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1674,100 +1653,9 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="37" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1778,6 +1666,100 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1796,8 +1778,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2123,8 +2106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CD4380-2153-411E-9E75-935A9463F7F9}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="D43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2132,64 +2115,64 @@
     <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="53" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="60.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="71.28515625" style="118" customWidth="1"/>
+    <col min="7" max="7" width="71.28515625" style="110" customWidth="1"/>
     <col min="8" max="11" width="22.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="26.42578125" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="103" t="s">
+      <c r="B1" s="121"/>
+      <c r="C1" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="113"/>
-      <c r="K1" s="155" t="s">
+      <c r="G1" s="105"/>
+      <c r="K1" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="156"/>
+      <c r="L1" s="119"/>
     </row>
     <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="158"/>
-      <c r="C2" s="104" t="s">
+      <c r="B2" s="121"/>
+      <c r="C2" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="113"/>
+      <c r="G2" s="105"/>
       <c r="K2" s="32" t="s">
         <v>22</v>
       </c>
       <c r="L2" s="29">
         <f>COUNTIF(L8:L364,"Passed")</f>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="157" t="s">
+      <c r="A3" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="158"/>
-      <c r="C3" s="104" t="s">
+      <c r="B3" s="121"/>
+      <c r="C3" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="113"/>
+      <c r="G3" s="105"/>
       <c r="K3" s="31" t="s">
         <v>20</v>
       </c>
@@ -2199,17 +2182,17 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="127"/>
+      <c r="C4" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="113"/>
+      <c r="G4" s="105"/>
       <c r="K4" s="30" t="s">
         <v>17</v>
       </c>
@@ -2219,17 +2202,17 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="140"/>
+      <c r="C5" s="136"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" s="114"/>
+      <c r="G5" s="106"/>
       <c r="H5"/>
       <c r="K5" s="28" t="s">
         <v>14</v>
@@ -2243,17 +2226,17 @@
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="86"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
-      <c r="G6" s="115"/>
+      <c r="G6" s="107"/>
       <c r="H6" s="25"/>
       <c r="K6" s="24" t="s">
         <v>13</v>
       </c>
       <c r="L6" s="23">
         <f>SUM(L2:L5)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2275,7 +2258,7 @@
       <c r="F7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="111" t="s">
+      <c r="G7" s="103" t="s">
         <v>28</v>
       </c>
       <c r="H7" s="21" t="s">
@@ -2295,615 +2278,675 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="92">
+      <c r="A8" s="84">
         <v>1</v>
       </c>
-      <c r="B8" s="129" t="s">
+      <c r="B8" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="123" t="s">
+      <c r="C8" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="135" t="s">
+      <c r="D8" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="141"/>
-      <c r="F8" s="105" t="s">
+      <c r="E8" s="137"/>
+      <c r="F8" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="63" t="s">
+      <c r="G8" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J8" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K8" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="93" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="84"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="97" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L9" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="84">
+        <v>2</v>
+      </c>
+      <c r="B10" s="124"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="104" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J10" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L10" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="84"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="129"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="138"/>
+      <c r="F11" s="99" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J11" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K11" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="84">
+        <v>3</v>
+      </c>
+      <c r="B12" s="124"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="138"/>
+      <c r="F12" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="108" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J12" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="84"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="146" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="133"/>
+      <c r="E13" s="138"/>
+      <c r="F13" s="101" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="109" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="I8" s="120" t="s">
+      <c r="I13" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J13" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="J8" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K8" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L8" s="42" t="s">
+      <c r="K13" s="114" t="s">
+        <v>133</v>
+      </c>
+      <c r="L13" s="113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="84">
+        <v>4</v>
+      </c>
+      <c r="B14" s="124"/>
+      <c r="C14" s="147"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="139"/>
+      <c r="F14" s="102" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K14" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L14" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="101" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="92"/>
-      <c r="B9" s="130"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="142"/>
-      <c r="F9" s="105" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="63" t="s">
+    <row r="15" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="84">
+        <v>5</v>
+      </c>
+      <c r="B15" s="124"/>
+      <c r="C15" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="131" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="140"/>
+      <c r="F15" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I9" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J9" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K9" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L9" s="42" t="s">
+      <c r="H15" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K15" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L15" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="92">
-        <v>2</v>
-      </c>
-      <c r="B10" s="130"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="106" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="112" t="s">
+    <row r="16" spans="1:12" s="111" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="84"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="129"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="141"/>
+      <c r="F16" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K16" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="84">
+        <v>6</v>
+      </c>
+      <c r="B17" s="124"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K17" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L17" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="84">
+        <v>7</v>
+      </c>
+      <c r="B18" s="124"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J18" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K18" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L18" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="84">
+        <v>8</v>
+      </c>
+      <c r="B19" s="124"/>
+      <c r="C19" s="128" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="132"/>
+      <c r="E19" s="141"/>
+      <c r="F19" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J19" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K19" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="84"/>
+      <c r="B20" s="124"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J20" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K20" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L20" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="84"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J21" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K21" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="84">
+        <v>9</v>
+      </c>
+      <c r="B22" s="124"/>
+      <c r="C22" s="130"/>
+      <c r="D22" s="148"/>
+      <c r="E22" s="142"/>
+      <c r="F22" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J22" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K22" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="84">
+        <v>10</v>
+      </c>
+      <c r="B23" s="124"/>
+      <c r="C23" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="143"/>
+      <c r="F23" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J23" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K23" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L23" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="84">
+        <v>11</v>
+      </c>
+      <c r="B24" s="124"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="150"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I10" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J10" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K10" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L10" s="42" t="s">
+      <c r="H24" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J24" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K24" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L24" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
-      <c r="B11" s="130"/>
-      <c r="C11" s="125"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="142"/>
-      <c r="F11" s="107" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="112" t="s">
-        <v>82</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I11" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J11" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K11" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L11" s="42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="92">
-        <v>3</v>
-      </c>
-      <c r="B12" s="130"/>
-      <c r="C12" s="124"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="142"/>
-      <c r="F12" s="108" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="116" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I12" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J12" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K12" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L12" s="42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="92"/>
-      <c r="B13" s="130"/>
-      <c r="C13" s="150" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="137"/>
-      <c r="E13" s="142"/>
-      <c r="F13" s="109" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="117" t="s">
-        <v>106</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="I13" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J13" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="K13" s="122" t="s">
-        <v>134</v>
-      </c>
-      <c r="L13" s="121" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="92">
-        <v>4</v>
-      </c>
-      <c r="B14" s="130"/>
-      <c r="C14" s="151"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="143"/>
-      <c r="F14" s="110" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I14" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J14" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K14" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L14" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="92">
-        <v>5</v>
-      </c>
-      <c r="B15" s="130"/>
-      <c r="C15" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="135" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="144"/>
-      <c r="F15" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I15" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J15" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K15" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L15" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="119" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
-      <c r="B16" s="130"/>
-      <c r="C16" s="125"/>
-      <c r="D16" s="136"/>
-      <c r="E16" s="145"/>
-      <c r="F16" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="G16" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I16" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J16" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K16" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L16" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92">
-        <v>6</v>
-      </c>
-      <c r="B17" s="130"/>
-      <c r="C17" s="125"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I17" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J17" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K17" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L17" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="92">
-        <v>7</v>
-      </c>
-      <c r="B18" s="130"/>
-      <c r="C18" s="124"/>
-      <c r="D18" s="136"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="H18" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I18" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J18" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K18" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L18" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="92">
-        <v>8</v>
-      </c>
-      <c r="B19" s="130"/>
-      <c r="C19" s="123" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="136"/>
-      <c r="E19" s="145"/>
-      <c r="F19" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="63" t="s">
-        <v>110</v>
-      </c>
-      <c r="H19" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I19" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J19" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K19" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L19" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="130"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="136"/>
-      <c r="E20" s="145"/>
-      <c r="F20" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="H20" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I20" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J20" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K20" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L20" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="92"/>
-      <c r="B21" s="130"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="136"/>
-      <c r="E21" s="145"/>
-      <c r="F21" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="72" t="s">
-        <v>112</v>
-      </c>
-      <c r="H21" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I21" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J21" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K21" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L21" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="92">
-        <v>9</v>
-      </c>
-      <c r="B22" s="130"/>
-      <c r="C22" s="124"/>
-      <c r="D22" s="152"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" s="59" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I22" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="J22" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="K22" s="120" t="s">
-        <v>132</v>
-      </c>
-      <c r="L22" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="92">
-        <v>10</v>
-      </c>
-      <c r="B23" s="130"/>
-      <c r="C23" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="126" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="147"/>
-      <c r="F23" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="42"/>
-    </row>
-    <row r="24" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
-      <c r="B24" s="130"/>
-      <c r="C24" s="125"/>
-      <c r="D24" s="127"/>
-      <c r="E24" s="148"/>
-      <c r="F24" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="36"/>
-    </row>
     <row r="25" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="92">
-        <v>11</v>
-      </c>
-      <c r="B25" s="130"/>
-      <c r="C25" s="125"/>
-      <c r="D25" s="127"/>
-      <c r="E25" s="148"/>
+      <c r="A25" s="84">
+        <v>12</v>
+      </c>
+      <c r="B25" s="124"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="144"/>
       <c r="F25" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="G25" s="112" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="7"/>
+      <c r="G25" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J25" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K25" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L25" s="59" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="92">
-        <v>12</v>
-      </c>
-      <c r="B26" s="130"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="127"/>
-      <c r="E26" s="148"/>
-      <c r="F26" s="15" t="s">
+      <c r="A26" s="84">
+        <v>13</v>
+      </c>
+      <c r="B26" s="124"/>
+      <c r="C26" s="130"/>
+      <c r="D26" s="150"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J26" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K26" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L26" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="115" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="84"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="160"/>
+      <c r="D27" s="150"/>
+      <c r="E27" s="144"/>
+      <c r="F27" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I27" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J27" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K27" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L27" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="84">
+        <v>14</v>
+      </c>
+      <c r="B28" s="124"/>
+      <c r="C28" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="151"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="7"/>
-    </row>
-    <row r="27" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="92">
-        <v>13</v>
-      </c>
-      <c r="B27" s="130"/>
-      <c r="C27" s="124"/>
-      <c r="D27" s="127"/>
-      <c r="E27" s="148"/>
-      <c r="F27" s="68" t="s">
+      <c r="H28" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="J28" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="K28" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="L28" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="84">
+        <v>15</v>
+      </c>
+      <c r="B29" s="124"/>
+      <c r="C29" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="149" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="51"/>
+      <c r="F29" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="G27" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="92">
-        <v>14</v>
-      </c>
-      <c r="B28" s="130"/>
-      <c r="C28" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="128"/>
-      <c r="E28" s="149"/>
-      <c r="F28" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="62"/>
-    </row>
-    <row r="29" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="92">
-        <v>15</v>
-      </c>
-      <c r="B29" s="130"/>
-      <c r="C29" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="126" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="56"/>
-      <c r="F29" s="37" t="s">
+      <c r="G29" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="38"/>
+    </row>
+    <row r="30" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="84">
+        <v>16</v>
+      </c>
+      <c r="B30" s="124"/>
+      <c r="C30" s="129"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="15" t="s">
         <v>101</v>
-      </c>
-      <c r="G29" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="42"/>
-    </row>
-    <row r="30" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="92">
-        <v>16</v>
-      </c>
-      <c r="B30" s="130"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="127"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="15" t="s">
-        <v>102</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>81</v>
@@ -2915,15 +2958,15 @@
       <c r="L30" s="7"/>
     </row>
     <row r="31" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="92">
+      <c r="A31" s="84">
         <v>17</v>
       </c>
-      <c r="B31" s="130"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="127"/>
-      <c r="E31" s="43"/>
+      <c r="B31" s="124"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="150"/>
+      <c r="E31" s="39"/>
       <c r="F31" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>82</v>
@@ -2935,15 +2978,15 @@
       <c r="L31" s="7"/>
     </row>
     <row r="32" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="93">
+      <c r="A32" s="85">
         <v>18</v>
       </c>
-      <c r="B32" s="130"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="127"/>
-      <c r="E32" s="43"/>
+      <c r="B32" s="124"/>
+      <c r="C32" s="129"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>82</v>
@@ -2955,18 +2998,18 @@
       <c r="L32" s="7"/>
     </row>
     <row r="33" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="93">
+      <c r="A33" s="85">
         <v>19</v>
       </c>
-      <c r="B33" s="130"/>
-      <c r="C33" s="124"/>
-      <c r="D33" s="128"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" s="46" t="s">
-        <v>116</v>
+      <c r="B33" s="124"/>
+      <c r="C33" s="130"/>
+      <c r="D33" s="151"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>115</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="4"/>
@@ -2975,40 +3018,40 @@
       <c r="L33" s="3"/>
     </row>
     <row r="34" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="93">
+      <c r="A34" s="85">
         <v>20</v>
       </c>
-      <c r="B34" s="130"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="126" t="s">
+      <c r="B34" s="124"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="149" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="56"/>
-      <c r="F34" s="87" t="s">
+      <c r="E34" s="51"/>
+      <c r="F34" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="G34" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="H34" s="88"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="42"/>
+      <c r="G34" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="H34" s="80"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="38"/>
     </row>
     <row r="35" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="93">
+      <c r="A35" s="85">
         <v>21</v>
       </c>
-      <c r="B35" s="130"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="127"/>
-      <c r="E35" s="43"/>
+      <c r="B35" s="124"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="150"/>
+      <c r="E35" s="39"/>
       <c r="F35" s="12" t="s">
         <v>68</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="8"/>
@@ -3017,20 +3060,20 @@
       <c r="L35" s="7"/>
     </row>
     <row r="36" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="93">
+      <c r="A36" s="85">
         <v>22</v>
       </c>
-      <c r="B36" s="130"/>
-      <c r="C36" s="90" t="s">
+      <c r="B36" s="124"/>
+      <c r="C36" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="43"/>
+      <c r="D36" s="150"/>
+      <c r="E36" s="39"/>
       <c r="F36" s="12" t="s">
         <v>69</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="8"/>
@@ -3039,18 +3082,18 @@
       <c r="L36" s="7"/>
     </row>
     <row r="37" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="93">
+      <c r="A37" s="85">
         <v>23</v>
       </c>
-      <c r="B37" s="130"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="127"/>
-      <c r="E37" s="43"/>
+      <c r="B37" s="124"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="39"/>
       <c r="F37" s="12" t="s">
         <v>70</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="8"/>
@@ -3059,18 +3102,18 @@
       <c r="L37" s="7"/>
     </row>
     <row r="38" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="93">
+      <c r="A38" s="85">
         <v>24</v>
       </c>
-      <c r="B38" s="130"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="89" t="s">
+      <c r="B38" s="124"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="151"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="81" t="s">
         <v>71</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="4"/>
@@ -3079,153 +3122,153 @@
       <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="93">
+      <c r="A39" s="85">
         <v>25</v>
       </c>
-      <c r="B39" s="130"/>
-      <c r="C39" s="123" t="s">
+      <c r="B39" s="124"/>
+      <c r="C39" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="126" t="s">
+      <c r="D39" s="149" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57" t="s">
+      <c r="E39" s="51"/>
+      <c r="F39" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="G39" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="H39" s="88"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="42"/>
+      <c r="G39" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H39" s="80"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="38"/>
     </row>
     <row r="40" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="93"/>
-      <c r="B40" s="130"/>
-      <c r="C40" s="124"/>
-      <c r="D40" s="128"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="91" t="s">
+      <c r="A40" s="85"/>
+      <c r="B40" s="124"/>
+      <c r="C40" s="130"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="G40" s="40" t="s">
+      <c r="G40" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="H40" s="96"/>
-      <c r="I40" s="97"/>
-      <c r="J40" s="97"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="52"/>
+      <c r="H40" s="88"/>
+      <c r="I40" s="89"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="47"/>
     </row>
     <row r="41" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="93"/>
-      <c r="B41" s="130"/>
-      <c r="C41" s="123" t="s">
+      <c r="A41" s="85"/>
+      <c r="B41" s="124"/>
+      <c r="C41" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="153" t="s">
+      <c r="D41" s="152" t="s">
         <v>76</v>
       </c>
-      <c r="E41" s="165"/>
-      <c r="F41" s="98" t="s">
+      <c r="E41" s="116"/>
+      <c r="F41" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="G41" s="40" t="s">
+      <c r="G41" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="H41" s="99"/>
-      <c r="I41" s="100"/>
-      <c r="J41" s="100"/>
-      <c r="K41" s="65"/>
-      <c r="L41" s="66"/>
+      <c r="H41" s="91"/>
+      <c r="I41" s="92"/>
+      <c r="J41" s="92"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="58"/>
     </row>
     <row r="42" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="93"/>
-      <c r="B42" s="130"/>
-      <c r="C42" s="124"/>
-      <c r="D42" s="154"/>
-      <c r="E42" s="166"/>
-      <c r="F42" s="91" t="s">
+      <c r="A42" s="85"/>
+      <c r="B42" s="124"/>
+      <c r="C42" s="130"/>
+      <c r="D42" s="153"/>
+      <c r="E42" s="117"/>
+      <c r="F42" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="G42" s="59" t="s">
+      <c r="G42" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="H42" s="96"/>
-      <c r="I42" s="97"/>
-      <c r="J42" s="97"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="52"/>
+      <c r="H42" s="88"/>
+      <c r="I42" s="89"/>
+      <c r="J42" s="89"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="47"/>
     </row>
     <row r="43" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="93"/>
-      <c r="B43" s="130"/>
-      <c r="C43" s="54"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="124"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="16"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="72"/>
-      <c r="H43" s="94"/>
-      <c r="I43" s="95"/>
-      <c r="J43" s="95"/>
-      <c r="K43" s="73"/>
-      <c r="L43" s="74"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="86"/>
+      <c r="I43" s="87"/>
+      <c r="J43" s="87"/>
+      <c r="K43" s="65"/>
+      <c r="L43" s="66"/>
     </row>
     <row r="44" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="93"/>
-      <c r="B44" s="130"/>
-      <c r="C44" s="54"/>
+      <c r="A44" s="85"/>
+      <c r="B44" s="124"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="16"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="91"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="94"/>
-      <c r="I44" s="95"/>
-      <c r="J44" s="95"/>
-      <c r="K44" s="73"/>
-      <c r="L44" s="74"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="86"/>
+      <c r="I44" s="87"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="65"/>
+      <c r="L44" s="66"/>
     </row>
     <row r="45" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="93"/>
-      <c r="B45" s="130"/>
-      <c r="C45" s="54"/>
+      <c r="A45" s="85"/>
+      <c r="B45" s="124"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="16"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="94"/>
-      <c r="I45" s="95"/>
-      <c r="J45" s="95"/>
-      <c r="K45" s="73"/>
-      <c r="L45" s="74"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="86"/>
+      <c r="I45" s="87"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="65"/>
+      <c r="L45" s="66"/>
     </row>
     <row r="46" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="93"/>
-      <c r="B46" s="130"/>
-      <c r="C46" s="54"/>
+      <c r="A46" s="85"/>
+      <c r="B46" s="124"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="16"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="91"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="94"/>
-      <c r="I46" s="95"/>
-      <c r="J46" s="95"/>
-      <c r="K46" s="73"/>
-      <c r="L46" s="74"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="86"/>
+      <c r="I46" s="87"/>
+      <c r="J46" s="87"/>
+      <c r="K46" s="65"/>
+      <c r="L46" s="66"/>
     </row>
     <row r="47" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="93">
+      <c r="A47" s="85">
         <v>26</v>
       </c>
-      <c r="B47" s="131"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="91"/>
-      <c r="G47" s="46"/>
+      <c r="B47" s="125"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="83"/>
+      <c r="G47" s="42"/>
       <c r="H47" s="6"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -3234,13 +3277,12 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C39:C40"/>
     <mergeCell ref="B8:B47"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D4:E4"/>
@@ -3253,16 +3295,17 @@
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="C19:C22"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C23:C26"/>
     <mergeCell ref="D15:D22"/>
     <mergeCell ref="D23:D28"/>
     <mergeCell ref="D41:D42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="D29:D33"/>
-    <mergeCell ref="D34:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="L8:L47">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -3287,20 +3330,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E83DD8F-1B30-4A24-875F-463EA716463A}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="85" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="77" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" style="76" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" style="68" customWidth="1"/>
     <col min="4" max="14" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="67" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="20" t="s">
@@ -3314,248 +3357,248 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="161">
+      <c r="A2" s="156">
         <v>1</v>
       </c>
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="154" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="75"/>
+    </row>
+    <row r="3" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="158"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="76"/>
+    </row>
+    <row r="4" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="158"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="76"/>
+    </row>
+    <row r="5" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="157"/>
+      <c r="B5" s="159"/>
+      <c r="C5" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="76"/>
+    </row>
+    <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="156">
+        <v>2</v>
+      </c>
+      <c r="B6" s="154" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="75"/>
+    </row>
+    <row r="7" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="158"/>
+      <c r="B7" s="159"/>
+      <c r="C7" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="76"/>
+    </row>
+    <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="158"/>
+      <c r="B8" s="159"/>
+      <c r="C8" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="76"/>
+    </row>
+    <row r="9" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="158"/>
+      <c r="B9" s="159"/>
+      <c r="C9" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="76"/>
+    </row>
+    <row r="10" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="158"/>
+      <c r="B10" s="159"/>
+      <c r="C10" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="157"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="73" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="76"/>
+    </row>
+    <row r="12" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="156">
+        <v>3</v>
+      </c>
+      <c r="B12" s="154" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="83"/>
-    </row>
-    <row r="3" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="163"/>
-      <c r="B3" s="164"/>
-      <c r="C3" s="79" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="84"/>
-    </row>
-    <row r="4" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="163"/>
-      <c r="B4" s="164"/>
-      <c r="C4" s="79" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="84"/>
-    </row>
-    <row r="5" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="162"/>
-      <c r="B5" s="164"/>
-      <c r="C5" s="79" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="84"/>
-    </row>
-    <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="161">
-        <v>2</v>
-      </c>
-      <c r="B6" s="159" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="83"/>
-    </row>
-    <row r="7" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="163"/>
-      <c r="B7" s="164"/>
-      <c r="C7" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="84"/>
-    </row>
-    <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="163"/>
-      <c r="B8" s="164"/>
-      <c r="C8" s="79" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="84"/>
-    </row>
-    <row r="9" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="163"/>
-      <c r="B9" s="164"/>
-      <c r="C9" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="84"/>
-    </row>
-    <row r="10" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="163"/>
-      <c r="B10" s="164"/>
-      <c r="C10" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="84"/>
-    </row>
-    <row r="11" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="162"/>
-      <c r="B11" s="164"/>
-      <c r="C11" s="81" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="84"/>
-    </row>
-    <row r="12" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="161">
-        <v>3</v>
-      </c>
-      <c r="B12" s="159" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="78"/>
+      <c r="D12" s="70"/>
     </row>
     <row r="13" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="163"/>
-      <c r="B13" s="164"/>
-      <c r="C13" s="79" t="s">
+      <c r="A13" s="158"/>
+      <c r="B13" s="159"/>
+      <c r="C13" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="80"/>
+      <c r="D13" s="72"/>
     </row>
     <row r="14" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="163"/>
-      <c r="B14" s="164"/>
-      <c r="C14" s="79" t="s">
+      <c r="A14" s="158"/>
+      <c r="B14" s="159"/>
+      <c r="C14" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="80"/>
+      <c r="D14" s="72"/>
     </row>
     <row r="15" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
-      <c r="B15" s="164"/>
-      <c r="C15" s="79" t="s">
+      <c r="A15" s="158"/>
+      <c r="B15" s="159"/>
+      <c r="C15" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="80"/>
+      <c r="D15" s="72"/>
     </row>
     <row r="16" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="162"/>
-      <c r="B16" s="160"/>
-      <c r="C16" s="81" t="s">
+      <c r="A16" s="157"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="82"/>
+      <c r="D16" s="74"/>
     </row>
     <row r="17" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="161">
+      <c r="A17" s="156">
         <v>4</v>
       </c>
-      <c r="B17" s="159" t="s">
+      <c r="B17" s="154" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="78"/>
+      <c r="D17" s="70"/>
     </row>
     <row r="18" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="163"/>
-      <c r="B18" s="164"/>
-      <c r="C18" s="79" t="s">
+      <c r="A18" s="158"/>
+      <c r="B18" s="159"/>
+      <c r="C18" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="80"/>
+      <c r="D18" s="72"/>
     </row>
     <row r="19" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="163"/>
-      <c r="B19" s="164"/>
-      <c r="C19" s="79" t="s">
+      <c r="A19" s="158"/>
+      <c r="B19" s="159"/>
+      <c r="C19" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="80"/>
+      <c r="D19" s="72"/>
     </row>
     <row r="20" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="163"/>
-      <c r="B20" s="164"/>
-      <c r="C20" s="79" t="s">
+      <c r="A20" s="158"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="80"/>
+      <c r="D20" s="72"/>
     </row>
     <row r="21" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="161">
+      <c r="A21" s="156">
         <v>5</v>
       </c>
-      <c r="B21" s="159" t="s">
+      <c r="B21" s="154" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="78"/>
+      <c r="D21" s="70"/>
     </row>
     <row r="22" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="163"/>
-      <c r="B22" s="164"/>
-      <c r="C22" s="79" t="s">
+      <c r="A22" s="158"/>
+      <c r="B22" s="159"/>
+      <c r="C22" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="80"/>
+      <c r="D22" s="72"/>
     </row>
     <row r="23" spans="1:4" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="162"/>
-      <c r="B23" s="160"/>
-      <c r="C23" s="81" t="s">
+      <c r="A23" s="157"/>
+      <c r="B23" s="155"/>
+      <c r="C23" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="82"/>
+      <c r="D23" s="74"/>
     </row>
     <row r="24" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="161">
+      <c r="A24" s="156">
         <v>5</v>
       </c>
-      <c r="B24" s="159" t="s">
+      <c r="B24" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="77" t="s">
+      <c r="C24" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="78"/>
+      <c r="D24" s="70"/>
     </row>
     <row r="25" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="163"/>
-      <c r="B25" s="164"/>
-      <c r="C25" s="79" t="s">
+      <c r="A25" s="158"/>
+      <c r="B25" s="159"/>
+      <c r="C25" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="80"/>
+      <c r="D25" s="72"/>
     </row>
     <row r="26" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="162"/>
-      <c r="B26" s="160"/>
-      <c r="C26" s="81" t="s">
+      <c r="A26" s="157"/>
+      <c r="B26" s="155"/>
+      <c r="C26" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="82"/>
+      <c r="D26" s="74"/>
     </row>
     <row r="27" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="161">
+      <c r="A27" s="156">
         <v>6</v>
       </c>
-      <c r="B27" s="159" t="s">
+      <c r="B27" s="154" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="C27" s="77" t="s">
+      <c r="D27" s="70"/>
+    </row>
+    <row r="28" spans="1:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="157"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="73" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="78"/>
-    </row>
-    <row r="28" spans="1:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="162"/>
-      <c r="B28" s="160"/>
-      <c r="C28" s="81" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" s="82"/>
+      <c r="D28" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
edit test cases status for checkbox
</commit_message>
<xml_diff>
--- a/TestDocuments/TestCases.xlsx
+++ b/TestDocuments/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quality Assurance\Workings\Automated Test\RahulshettyPractice\RahulShettyAcademyAutomatedTest\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9092F9CF-D093-4C88-AB4E-8C82EA98AD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAD48DD-7BF5-4686-B59C-E98A638B64BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Elements" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="137">
   <si>
     <t>Functional Testing</t>
   </si>
@@ -350,9 +350,6 @@
     <t>Verifying checkboxes by their label and value</t>
   </si>
   <si>
-    <t>Verifying checkboxes are selectable</t>
-  </si>
-  <si>
     <t>Verifying multiple checkboxes are selectable at once</t>
   </si>
   <si>
@@ -453,6 +450,9 @@
   </si>
   <si>
     <t xml:space="preserve">Should not be selectable </t>
+  </si>
+  <si>
+    <t>Verifying clicking checkbox selects option</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1327,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1357,9 +1357,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1425,9 +1422,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1656,6 +1650,103 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1666,100 +1757,6 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1776,9 +1773,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2106,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CD4380-2153-411E-9E75-935A9463F7F9}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView topLeftCell="D43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="F31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2115,68 +2109,68 @@
     <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="53" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="51" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="60.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="71.28515625" style="110" customWidth="1"/>
+    <col min="7" max="7" width="71.28515625" style="108" customWidth="1"/>
     <col min="8" max="11" width="22.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="26.42578125" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="151" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="95" t="s">
+      <c r="B1" s="152"/>
+      <c r="C1" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="105"/>
-      <c r="K1" s="118" t="s">
+      <c r="G1" s="103"/>
+      <c r="K1" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="119"/>
+      <c r="L1" s="150"/>
     </row>
     <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="96" t="s">
+      <c r="B2" s="152"/>
+      <c r="C2" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="105"/>
-      <c r="K2" s="32" t="s">
+      <c r="G2" s="103"/>
+      <c r="K2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="29">
+      <c r="L2" s="28">
         <f>COUNTIF(L8:L364,"Passed")</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="151" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="152"/>
+      <c r="C3" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="103"/>
+      <c r="K3" s="30" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="120" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="96" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="105"/>
-      <c r="K3" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="29">
+      <c r="L3" s="28">
         <f>COUNTIF(L8:L711,"Failed")</f>
         <v>1</v>
       </c>
@@ -2186,872 +2180,922 @@
         <v>19</v>
       </c>
       <c r="B4" s="127"/>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="105"/>
-      <c r="K4" s="30" t="s">
+      <c r="G4" s="103"/>
+      <c r="K4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="28">
         <f>COUNTIF(L7:L711,"Not Executed")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="136"/>
+      <c r="C5" s="134"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" s="106"/>
+      <c r="G5" s="104"/>
       <c r="H5"/>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="26">
         <f>COUNTIF(L7:L711,"Out of Scope")</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="25"/>
-      <c r="K6" s="24" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="24"/>
+      <c r="K6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="22">
         <f>SUM(L2:L5)</f>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="103" t="s">
+      <c r="G7" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="84">
+      <c r="A8" s="82">
         <v>1</v>
       </c>
       <c r="B8" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="128" t="s">
+      <c r="C8" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="137"/>
-      <c r="F8" s="97" t="s">
+      <c r="E8" s="135"/>
+      <c r="F8" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="55" t="s">
+      <c r="G8" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J8" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K8" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="91" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="82"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="119"/>
+      <c r="D9" s="130"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="95" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J9" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K9" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="82">
+        <v>2</v>
+      </c>
+      <c r="B10" s="124"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J10" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K10" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="82"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="102" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J11" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L11" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="82">
+        <v>3</v>
+      </c>
+      <c r="B12" s="124"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="106" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="82"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="144" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="131"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="99" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="107" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="I8" s="112" t="s">
+      <c r="I13" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J13" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="J8" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K8" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L8" s="38" t="s">
+      <c r="K13" s="112" t="s">
+        <v>132</v>
+      </c>
+      <c r="L13" s="111" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="82">
+        <v>4</v>
+      </c>
+      <c r="B14" s="124"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="137"/>
+      <c r="F14" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I14" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K14" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L14" s="57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="93" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="124"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="97" t="s">
-        <v>124</v>
-      </c>
-      <c r="G9" s="55" t="s">
+    <row r="15" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="82">
+        <v>5</v>
+      </c>
+      <c r="B15" s="124"/>
+      <c r="C15" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="129" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="138"/>
+      <c r="F15" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I9" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J9" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K9" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L9" s="38" t="s">
+      <c r="H15" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I15" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J15" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L15" s="57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="84">
-        <v>2</v>
-      </c>
-      <c r="B10" s="124"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="98" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="104" t="s">
+    <row r="16" spans="1:12" s="109" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="82"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="130"/>
+      <c r="E16" s="139"/>
+      <c r="F16" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I16" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L16" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="82">
+        <v>6</v>
+      </c>
+      <c r="B17" s="124"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J17" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K17" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L17" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="82">
+        <v>7</v>
+      </c>
+      <c r="B18" s="124"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J18" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K18" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L18" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="82">
+        <v>8</v>
+      </c>
+      <c r="B19" s="124"/>
+      <c r="C19" s="117" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="130"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J19" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K19" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L19" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="82"/>
+      <c r="B20" s="124"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="130"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J20" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K20" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L20" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="82"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="130"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J21" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K21" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L21" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="82">
+        <v>9</v>
+      </c>
+      <c r="B22" s="124"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J22" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K22" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L22" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="82">
+        <v>10</v>
+      </c>
+      <c r="B23" s="124"/>
+      <c r="C23" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="120" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="141"/>
+      <c r="F23" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K23" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L23" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="82">
+        <v>11</v>
+      </c>
+      <c r="B24" s="124"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="142"/>
+      <c r="F24" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I10" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J10" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K10" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L10" s="38" t="s">
+      <c r="H24" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K24" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L24" s="57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="84"/>
-      <c r="B11" s="124"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="99" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="104" t="s">
+    <row r="25" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="82">
+        <v>12</v>
+      </c>
+      <c r="B25" s="124"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="142"/>
+      <c r="F25" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J25" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K25" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L25" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="82">
+        <v>13</v>
+      </c>
+      <c r="B26" s="124"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="H11" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I11" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J11" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K11" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L11" s="38" t="s">
+      <c r="H26" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K26" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L26" s="57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="84">
-        <v>3</v>
-      </c>
-      <c r="B12" s="124"/>
-      <c r="C12" s="130"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="100" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="108" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I12" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J12" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K12" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L12" s="38" t="s">
+    <row r="27" spans="1:12" s="113" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="82"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I27" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K27" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L27" s="57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="84"/>
-      <c r="B13" s="124"/>
-      <c r="C13" s="146" t="s">
+    <row r="28" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="82">
+        <v>14</v>
+      </c>
+      <c r="B28" s="124"/>
+      <c r="C28" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="133"/>
-      <c r="E13" s="138"/>
-      <c r="F13" s="101" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="109" t="s">
-        <v>105</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="I13" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J13" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="K13" s="114" t="s">
-        <v>133</v>
-      </c>
-      <c r="L13" s="113" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="84">
-        <v>4</v>
-      </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="147"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="139"/>
-      <c r="F14" s="102" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="54" t="s">
+      <c r="D28" s="122"/>
+      <c r="E28" s="143"/>
+      <c r="F28" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I28" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K28" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L28" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="82">
+        <v>15</v>
+      </c>
+      <c r="B29" s="124"/>
+      <c r="C29" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="49"/>
+      <c r="F29" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I29" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J29" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K29" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L29" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="82">
+        <v>16</v>
+      </c>
+      <c r="B30" s="124"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I30" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J30" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K30" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L30" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="82">
+        <v>17</v>
+      </c>
+      <c r="B31" s="124"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I14" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J14" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K14" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L14" s="59" t="s">
+      <c r="H31" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I31" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K31" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L31" s="57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="84">
-        <v>5</v>
-      </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="131" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="140"/>
-      <c r="F15" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J15" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K15" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L15" s="59" t="s">
+    <row r="32" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="83">
+        <v>18</v>
+      </c>
+      <c r="B32" s="124"/>
+      <c r="C32" s="119"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I32" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K32" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L32" s="57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="111" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="84"/>
-      <c r="B16" s="124"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="141"/>
-      <c r="F16" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="G16" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I16" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J16" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K16" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L16" s="59" t="s">
+    <row r="33" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="83">
+        <v>19</v>
+      </c>
+      <c r="B33" s="124"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="J33" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="K33" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="L33" s="57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="84">
-        <v>6</v>
-      </c>
-      <c r="B17" s="124"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="141"/>
-      <c r="F17" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I17" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J17" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K17" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L17" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="84">
-        <v>7</v>
-      </c>
-      <c r="B18" s="124"/>
-      <c r="C18" s="130"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I18" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J18" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K18" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L18" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="84">
-        <v>8</v>
-      </c>
-      <c r="B19" s="124"/>
-      <c r="C19" s="128" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="132"/>
-      <c r="E19" s="141"/>
-      <c r="F19" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I19" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J19" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K19" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L19" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="84"/>
-      <c r="B20" s="124"/>
-      <c r="C20" s="129"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I20" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J20" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K20" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L20" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="84"/>
-      <c r="B21" s="124"/>
-      <c r="C21" s="129"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="141"/>
-      <c r="F21" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="H21" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I21" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J21" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K21" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L21" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="84">
-        <v>9</v>
-      </c>
-      <c r="B22" s="124"/>
-      <c r="C22" s="130"/>
-      <c r="D22" s="148"/>
-      <c r="E22" s="142"/>
-      <c r="F22" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I22" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J22" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K22" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L22" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="84">
-        <v>10</v>
-      </c>
-      <c r="B23" s="124"/>
-      <c r="C23" s="128" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="149" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="143"/>
-      <c r="F23" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I23" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J23" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K23" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L23" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="84">
-        <v>11</v>
-      </c>
-      <c r="B24" s="124"/>
-      <c r="C24" s="129"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="104" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I24" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J24" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K24" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L24" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="84">
-        <v>12</v>
-      </c>
-      <c r="B25" s="124"/>
-      <c r="C25" s="129"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="H25" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I25" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J25" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K25" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L25" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="84">
-        <v>13</v>
-      </c>
-      <c r="B26" s="124"/>
-      <c r="C26" s="130"/>
-      <c r="D26" s="150"/>
-      <c r="E26" s="144"/>
-      <c r="F26" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I26" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J26" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K26" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L26" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="115" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="84"/>
-      <c r="B27" s="124"/>
-      <c r="C27" s="160"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="144"/>
-      <c r="F27" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="G27" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="H27" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I27" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J27" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K27" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L27" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="84">
-        <v>14</v>
-      </c>
-      <c r="B28" s="124"/>
-      <c r="C28" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="151"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="H28" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="I28" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="J28" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="K28" s="112" t="s">
-        <v>131</v>
-      </c>
-      <c r="L28" s="59" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="84">
-        <v>15</v>
-      </c>
-      <c r="B29" s="124"/>
-      <c r="C29" s="128" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="149" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="51"/>
-      <c r="F29" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="38"/>
-    </row>
-    <row r="30" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="84">
-        <v>16</v>
-      </c>
-      <c r="B30" s="124"/>
-      <c r="C30" s="129"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="7"/>
-    </row>
-    <row r="31" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="84">
-        <v>17</v>
-      </c>
-      <c r="B31" s="124"/>
-      <c r="C31" s="129"/>
-      <c r="D31" s="150"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="85">
-        <v>18</v>
-      </c>
-      <c r="B32" s="124"/>
-      <c r="C32" s="129"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="7"/>
-    </row>
-    <row r="33" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="85">
-        <v>19</v>
-      </c>
-      <c r="B33" s="124"/>
-      <c r="C33" s="130"/>
-      <c r="D33" s="151"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="G33" s="42" t="s">
+    <row r="34" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="83">
+        <v>20</v>
+      </c>
+      <c r="B34" s="124"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="120" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="49"/>
+      <c r="F34" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="H33" s="6"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="85">
-        <v>20</v>
-      </c>
-      <c r="B34" s="124"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="149" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="51"/>
-      <c r="F34" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="35" t="s">
+      <c r="H34" s="78"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="36"/>
+    </row>
+    <row r="35" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="83">
+        <v>21</v>
+      </c>
+      <c r="B35" s="124"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="H34" s="80"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="38"/>
-    </row>
-    <row r="35" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="85">
-        <v>21</v>
-      </c>
-      <c r="B35" s="124"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="150"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>117</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="8"/>
@@ -3060,20 +3104,20 @@
       <c r="L35" s="7"/>
     </row>
     <row r="36" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="85">
+      <c r="A36" s="83">
         <v>22</v>
       </c>
       <c r="B36" s="124"/>
-      <c r="C36" s="82" t="s">
+      <c r="C36" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="150"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="12" t="s">
+      <c r="D36" s="121"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="13" t="s">
-        <v>118</v>
+      <c r="G36" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="8"/>
@@ -3082,18 +3126,18 @@
       <c r="L36" s="7"/>
     </row>
     <row r="37" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="85">
+      <c r="A37" s="83">
         <v>23</v>
       </c>
       <c r="B37" s="124"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="150"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="12" t="s">
+      <c r="C37" s="41"/>
+      <c r="D37" s="121"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="11" t="s">
         <v>70</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="8"/>
@@ -3102,18 +3146,18 @@
       <c r="L37" s="7"/>
     </row>
     <row r="38" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="85">
+      <c r="A38" s="83">
         <v>24</v>
       </c>
       <c r="B38" s="124"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="151"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="81" t="s">
+      <c r="C38" s="42"/>
+      <c r="D38" s="122"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="79" t="s">
         <v>71</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="4"/>
@@ -3122,153 +3166,153 @@
       <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="85">
+      <c r="A39" s="83">
         <v>25</v>
       </c>
       <c r="B39" s="124"/>
-      <c r="C39" s="128" t="s">
+      <c r="C39" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="149" t="s">
+      <c r="D39" s="120" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="51"/>
-      <c r="F39" s="52" t="s">
+      <c r="E39" s="49"/>
+      <c r="F39" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="G39" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="H39" s="80"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="38"/>
+      <c r="G39" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="H39" s="78"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="36"/>
     </row>
     <row r="40" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="85"/>
+      <c r="A40" s="83"/>
       <c r="B40" s="124"/>
-      <c r="C40" s="130"/>
-      <c r="D40" s="151"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="83" t="s">
+      <c r="C40" s="118"/>
+      <c r="D40" s="122"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="G40" s="36" t="s">
+      <c r="G40" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="H40" s="88"/>
-      <c r="I40" s="89"/>
-      <c r="J40" s="89"/>
-      <c r="K40" s="46"/>
-      <c r="L40" s="47"/>
+      <c r="H40" s="86"/>
+      <c r="I40" s="87"/>
+      <c r="J40" s="87"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="45"/>
     </row>
     <row r="41" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="85"/>
+      <c r="A41" s="83"/>
       <c r="B41" s="124"/>
-      <c r="C41" s="128" t="s">
+      <c r="C41" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="152" t="s">
+      <c r="D41" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="E41" s="116"/>
-      <c r="F41" s="90" t="s">
+      <c r="E41" s="114"/>
+      <c r="F41" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="G41" s="36" t="s">
+      <c r="G41" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="H41" s="91"/>
-      <c r="I41" s="92"/>
-      <c r="J41" s="92"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="58"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="90"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="56"/>
     </row>
     <row r="42" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="85"/>
+      <c r="A42" s="83"/>
       <c r="B42" s="124"/>
-      <c r="C42" s="130"/>
-      <c r="D42" s="153"/>
-      <c r="E42" s="117"/>
-      <c r="F42" s="83" t="s">
+      <c r="C42" s="118"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="G42" s="54" t="s">
+      <c r="G42" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="H42" s="88"/>
-      <c r="I42" s="89"/>
-      <c r="J42" s="89"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="47"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="45"/>
     </row>
     <row r="43" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="85"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="124"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="83"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="86"/>
-      <c r="I43" s="87"/>
-      <c r="J43" s="87"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="66"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="81"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="84"/>
+      <c r="I43" s="85"/>
+      <c r="J43" s="85"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="64"/>
     </row>
     <row r="44" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="85"/>
+      <c r="A44" s="83"/>
       <c r="B44" s="124"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="83"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="86"/>
-      <c r="I44" s="87"/>
-      <c r="J44" s="87"/>
-      <c r="K44" s="65"/>
-      <c r="L44" s="66"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="81"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="84"/>
+      <c r="I44" s="85"/>
+      <c r="J44" s="85"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="64"/>
     </row>
     <row r="45" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="85"/>
+      <c r="A45" s="83"/>
       <c r="B45" s="124"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="83"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="86"/>
-      <c r="I45" s="87"/>
-      <c r="J45" s="87"/>
-      <c r="K45" s="65"/>
-      <c r="L45" s="66"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="81"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="84"/>
+      <c r="I45" s="85"/>
+      <c r="J45" s="85"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="64"/>
     </row>
     <row r="46" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="85"/>
+      <c r="A46" s="83"/>
       <c r="B46" s="124"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="86"/>
-      <c r="I46" s="87"/>
-      <c r="J46" s="87"/>
-      <c r="K46" s="65"/>
-      <c r="L46" s="66"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="81"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="84"/>
+      <c r="I46" s="85"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="64"/>
     </row>
     <row r="47" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="85">
+      <c r="A47" s="83">
         <v>26</v>
       </c>
       <c r="B47" s="125"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="83"/>
-      <c r="G47" s="42"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="81"/>
+      <c r="G47" s="40"/>
       <c r="H47" s="6"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -3277,12 +3321,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="D29:D33"/>
-    <mergeCell ref="D34:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
     <mergeCell ref="B8:B47"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D4:E4"/>
@@ -3299,13 +3344,12 @@
     <mergeCell ref="D15:D22"/>
     <mergeCell ref="D23:D28"/>
     <mergeCell ref="D41:D42"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <conditionalFormatting sqref="L8:L47">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -3330,275 +3374,275 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E83DD8F-1B30-4A24-875F-463EA716463A}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="77" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="75" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" style="68" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" style="66" customWidth="1"/>
     <col min="4" max="14" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="156">
+      <c r="A2" s="155">
         <v>1</v>
       </c>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="153" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="69" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="73"/>
+    </row>
+    <row r="3" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="157"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="74"/>
+    </row>
+    <row r="4" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="157"/>
+      <c r="B4" s="158"/>
+      <c r="C4" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="74"/>
+    </row>
+    <row r="5" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="156"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="74"/>
+    </row>
+    <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="155">
+        <v>2</v>
+      </c>
+      <c r="B6" s="153" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="73"/>
+    </row>
+    <row r="7" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="157"/>
+      <c r="B7" s="158"/>
+      <c r="C7" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="74"/>
+    </row>
+    <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="157"/>
+      <c r="B8" s="158"/>
+      <c r="C8" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="74"/>
+    </row>
+    <row r="9" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="157"/>
+      <c r="B9" s="158"/>
+      <c r="C9" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="74"/>
+    </row>
+    <row r="10" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="157"/>
+      <c r="B10" s="158"/>
+      <c r="C10" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="74"/>
+    </row>
+    <row r="11" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="156"/>
+      <c r="B11" s="158"/>
+      <c r="C11" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="74"/>
+    </row>
+    <row r="12" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="155">
+        <v>3</v>
+      </c>
+      <c r="B12" s="153" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="75"/>
-    </row>
-    <row r="3" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="158"/>
-      <c r="B3" s="159"/>
-      <c r="C3" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="76"/>
-    </row>
-    <row r="4" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="158"/>
-      <c r="B4" s="159"/>
-      <c r="C4" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="76"/>
-    </row>
-    <row r="5" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="157"/>
-      <c r="B5" s="159"/>
-      <c r="C5" s="71" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="76"/>
-    </row>
-    <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="156">
-        <v>2</v>
-      </c>
-      <c r="B6" s="154" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="75"/>
-    </row>
-    <row r="7" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="158"/>
-      <c r="B7" s="159"/>
-      <c r="C7" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="76"/>
-    </row>
-    <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="158"/>
-      <c r="B8" s="159"/>
-      <c r="C8" s="71" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="76"/>
-    </row>
-    <row r="9" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="158"/>
-      <c r="B9" s="159"/>
-      <c r="C9" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="76"/>
-    </row>
-    <row r="10" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="158"/>
-      <c r="B10" s="159"/>
-      <c r="C10" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="157"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="73" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="76"/>
-    </row>
-    <row r="12" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="156">
-        <v>3</v>
-      </c>
-      <c r="B12" s="154" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="70"/>
+      <c r="D12" s="68"/>
     </row>
     <row r="13" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="158"/>
-      <c r="B13" s="159"/>
-      <c r="C13" s="71" t="s">
+      <c r="A13" s="157"/>
+      <c r="B13" s="158"/>
+      <c r="C13" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="72"/>
+      <c r="D13" s="70"/>
     </row>
     <row r="14" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="158"/>
-      <c r="B14" s="159"/>
-      <c r="C14" s="71" t="s">
+      <c r="A14" s="157"/>
+      <c r="B14" s="158"/>
+      <c r="C14" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="72"/>
+      <c r="D14" s="70"/>
     </row>
     <row r="15" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="158"/>
-      <c r="B15" s="159"/>
-      <c r="C15" s="71" t="s">
+      <c r="A15" s="157"/>
+      <c r="B15" s="158"/>
+      <c r="C15" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="72"/>
+      <c r="D15" s="70"/>
     </row>
     <row r="16" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="157"/>
-      <c r="B16" s="155"/>
-      <c r="C16" s="73" t="s">
+      <c r="A16" s="156"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="74"/>
+      <c r="D16" s="72"/>
     </row>
     <row r="17" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="156">
+      <c r="A17" s="155">
         <v>4</v>
       </c>
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="70"/>
+      <c r="D17" s="68"/>
     </row>
     <row r="18" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="158"/>
-      <c r="B18" s="159"/>
-      <c r="C18" s="71" t="s">
+      <c r="A18" s="157"/>
+      <c r="B18" s="158"/>
+      <c r="C18" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="72"/>
+      <c r="D18" s="70"/>
     </row>
     <row r="19" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="158"/>
-      <c r="B19" s="159"/>
-      <c r="C19" s="71" t="s">
+      <c r="A19" s="157"/>
+      <c r="B19" s="158"/>
+      <c r="C19" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="72"/>
+      <c r="D19" s="70"/>
     </row>
     <row r="20" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="158"/>
-      <c r="B20" s="159"/>
-      <c r="C20" s="71" t="s">
+      <c r="A20" s="157"/>
+      <c r="B20" s="158"/>
+      <c r="C20" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="72"/>
+      <c r="D20" s="70"/>
     </row>
     <row r="21" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="156">
+      <c r="A21" s="155">
         <v>5</v>
       </c>
-      <c r="B21" s="154" t="s">
+      <c r="B21" s="153" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="70"/>
+      <c r="D21" s="68"/>
     </row>
     <row r="22" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="158"/>
-      <c r="B22" s="159"/>
-      <c r="C22" s="71" t="s">
+      <c r="A22" s="157"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="72"/>
+      <c r="D22" s="70"/>
     </row>
     <row r="23" spans="1:4" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="157"/>
-      <c r="B23" s="155"/>
-      <c r="C23" s="73" t="s">
+      <c r="A23" s="156"/>
+      <c r="B23" s="154"/>
+      <c r="C23" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="74"/>
+      <c r="D23" s="72"/>
     </row>
     <row r="24" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="156">
+      <c r="A24" s="155">
         <v>5</v>
       </c>
-      <c r="B24" s="154" t="s">
+      <c r="B24" s="153" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="69" t="s">
+      <c r="C24" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="70"/>
+      <c r="D24" s="68"/>
     </row>
     <row r="25" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="158"/>
-      <c r="B25" s="159"/>
-      <c r="C25" s="71" t="s">
+      <c r="A25" s="157"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="72"/>
+      <c r="D25" s="70"/>
     </row>
     <row r="26" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="157"/>
-      <c r="B26" s="155"/>
-      <c r="C26" s="73" t="s">
+      <c r="A26" s="156"/>
+      <c r="B26" s="154"/>
+      <c r="C26" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="74"/>
+      <c r="D26" s="72"/>
     </row>
     <row r="27" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="156">
+      <c r="A27" s="155">
         <v>6</v>
       </c>
-      <c r="B27" s="154" t="s">
+      <c r="B27" s="153" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="67" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="69" t="s">
+      <c r="D27" s="68"/>
+    </row>
+    <row r="28" spans="1:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="156"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="D27" s="70"/>
-    </row>
-    <row r="28" spans="1:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="157"/>
-      <c r="B28" s="155"/>
-      <c r="C28" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="74"/>
+      <c r="D28" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>